<commit_message>
Advance filters Pivot Table
</commit_message>
<xml_diff>
--- a/Excel/7. Xlookup/Lecture_XLookup_Solved.xlsx
+++ b/Excel/7. Xlookup/Lecture_XLookup_Solved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advance_Excel_BI\7. Xlookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC_DDS_02\Excel\7. Xlookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AC95AE-405A-49C8-A31F-1CA29FDFFC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B63CC6-A801-48CF-A8FC-2C24FB960927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="797" activeTab="6" xr2:uid="{00531900-100F-4AA3-B49D-7ADCF6C07589}"/>
   </bookViews>
@@ -231,12 +231,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="###"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +262,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,11 +489,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,13 +551,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{71786D01-B5CB-4281-852B-88DC3C8B88DB}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -65791,7 +65804,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66017,7 +66030,7 @@
       <c r="C15" s="7">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G15" t="s">
@@ -66094,6 +66107,9 @@
   <mergeCells count="1">
     <mergeCell ref="E8:J13"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E15" r:id="rId1" xr:uid="{8A2320A8-C274-4F7C-841D-D9AF254E43E2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>